<commit_message>
Updated some errors, removed interactive plot script, and made a shiny app
</commit_message>
<xml_diff>
--- a/outputs/data/dataset.xlsx
+++ b/outputs/data/dataset.xlsx
@@ -35,7 +35,7 @@
     <t>Freedom to make life choices - 2020</t>
   </si>
   <si>
-    <t>Generocity - 2020</t>
+    <t>Generosity - 2020</t>
   </si>
   <si>
     <t>Perceptions of Corruption - 2020</t>
@@ -56,7 +56,7 @@
     <t>Freedom to make life choices - 2021</t>
   </si>
   <si>
-    <t>Generocity - 2021</t>
+    <t>Generosity - 2021</t>
   </si>
   <si>
     <t>Perceptions of Corruption - 2021</t>

</xml_diff>